<commit_message>
add UBNT related automation script
</commit_message>
<xml_diff>
--- a/src/main/java/testData/testData_UBNT.xlsx
+++ b/src/main/java/testData/testData_UBNT.xlsx
@@ -16,16 +16,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
   <si>
     <t>1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>TrainScheduling_ltrailways_login_master</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Login.login</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -38,10 +34,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>TrainScheduling_ltrailways_login_master</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>country</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -62,7 +54,111 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>UBNT_configuration</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>false</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>840</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tabName1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>W</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wirelessMode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ap</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chanelWidth</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SSID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>xmtd1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>frequency</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2437</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AntennaGain</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>outputPower</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>25</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>newPassword</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>xalt12345</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tabName2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>updatedIPAddress</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10.1.2.103</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>updatedNetmask</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>255.255.248.0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10.1.2.1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gatewayIP</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -132,7 +228,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -144,6 +240,8 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -438,81 +536,160 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11:C12"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.95" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="35.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18" style="1" customWidth="1"/>
     <col min="2" max="2" width="4" style="1" customWidth="1"/>
     <col min="3" max="3" width="9.875" style="1" customWidth="1"/>
     <col min="4" max="4" width="10.375" style="1" customWidth="1"/>
     <col min="5" max="5" width="9.25" style="1" customWidth="1"/>
     <col min="6" max="6" width="7.875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="18.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9" style="1"/>
+    <col min="7" max="7" width="8.875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="13.75" style="1" customWidth="1"/>
+    <col min="9" max="9" width="9.875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="7.125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="12.375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="9.375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="11.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9" style="1"/>
+    <col min="18" max="18" width="16.625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="16" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" ht="15.95" customHeight="1"/>
-    <row r="2" spans="1:8" s="5" customFormat="1" ht="15.95" customHeight="1">
+    <row r="1" spans="1:20" s="2" customFormat="1" ht="15.95" customHeight="1"/>
+    <row r="2" spans="1:20" s="5" customFormat="1" ht="15.95" customHeight="1">
       <c r="A2" s="5" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="5" t="s">
-        <v>10</v>
+      <c r="I2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="P2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q2" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="R2" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="S2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="T2" s="8" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="3" customFormat="1" ht="15.95" customHeight="1">
+    <row r="3" spans="1:20" s="3" customFormat="1" ht="15.95" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="3">
-        <v>840</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>9</v>
-      </c>
       <c r="H3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O3" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="P3" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="R3" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="S3" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="T3" s="7" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add 'UBNT_M2' automation script
</commit_message>
<xml_diff>
--- a/src/main/java/testData/testData_UBNT.xlsx
+++ b/src/main/java/testData/testData_UBNT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
   <si>
     <t>1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -159,6 +159,14 @@
   </si>
   <si>
     <t>gatewayIP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tabName3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>U</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -536,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T3"/>
+  <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.95" customHeight="1"/>
@@ -567,8 +575,8 @@
     <col min="21" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="2" customFormat="1" ht="15.95" customHeight="1"/>
-    <row r="2" spans="1:20" s="5" customFormat="1" ht="15.95" customHeight="1">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15.95" customHeight="1"/>
+    <row r="2" spans="1:21" s="5" customFormat="1" ht="15.95" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>9</v>
       </c>
@@ -629,8 +637,11 @@
       <c r="T2" s="8" t="s">
         <v>35</v>
       </c>
+      <c r="U2" s="8" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="3" spans="1:20" s="3" customFormat="1" ht="15.95" customHeight="1">
+    <row r="3" spans="1:21" s="3" customFormat="1" ht="15.95" customHeight="1">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -643,7 +654,7 @@
       <c r="D3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="7" t="s">
         <v>5</v>
       </c>
       <c r="F3" s="3" t="s">
@@ -690,6 +701,9 @@
       </c>
       <c r="T3" s="7" t="s">
         <v>34</v>
+      </c>
+      <c r="U3" s="7" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>